<commit_message>
created R script to import previous work
</commit_message>
<xml_diff>
--- a/previous_work/CIRPinst-2011-2015-exclude.xlsx
+++ b/previous_work/CIRPinst-2011-2015-exclude.xlsx
@@ -8,22 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Departments/Institutional Research/Student-Research-Assistant/Shulav/GradRate_reg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F62D89-1F65-3348-AA45-68942FE3EB08}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12CFE3A-9709-0544-ADC7-6647FAA5848A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="460" windowWidth="20940" windowHeight="21060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="180" yWindow="460" windowWidth="20940" windowHeight="21060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2011-2015" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId1"/>
+    <sheet name="2011-2015" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2011-2015'!$A$1:$D$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2011-2015'!$A$1:$H$1</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
+  <pivotCaches>
+    <pivotCache cacheId="10" r:id="rId3"/>
+  </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="95">
   <si>
     <t>Harvey Mudd College</t>
   </si>
@@ -250,6 +254,12 @@
     <t>ACE</t>
   </si>
   <si>
+    <t>count name in Shulav data</t>
+  </si>
+  <si>
+    <t>apostrophe</t>
+  </si>
+  <si>
     <t>Alt name</t>
   </si>
   <si>
@@ -263,6 +273,45 @@
   </si>
   <si>
     <t>UnitID</t>
+  </si>
+  <si>
+    <t>BASIC2018</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Associate's Colleges: High Transfer-High Traditional</t>
+  </si>
+  <si>
+    <t>Baccalaureate Colleges: Arts &amp; Sciences Focus</t>
+  </si>
+  <si>
+    <t>Baccalaureate Colleges: Diverse Fields</t>
+  </si>
+  <si>
+    <t>Doctoral/Professional Universities</t>
+  </si>
+  <si>
+    <t>Master's Colleges &amp; Universities: Larger Programs</t>
+  </si>
+  <si>
+    <t>Master's Colleges &amp; Universities: Medium Programs</t>
+  </si>
+  <si>
+    <t>Master's Colleges &amp; Universities: Small Programs</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Count of UnitID</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Carnegie Classification</t>
   </si>
 </sst>
 </file>
@@ -306,10 +355,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -325,6 +382,1156 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ellen Kotler" refreshedDate="43616.38222349537" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="70" xr:uid="{E0C2B4B8-DA30-AF4E-98EC-4F6A916D8CC6}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:H71" sheet="2011-2015"/>
+  </cacheSource>
+  <cacheFields count="8">
+    <cacheField name="Institution" numFmtId="0">
+      <sharedItems count="70">
+        <s v="Agnes Scott College"/>
+        <s v="Albion College"/>
+        <s v="Allegheny College"/>
+        <s v="Alma College"/>
+        <s v="Belmont University"/>
+        <s v="Beloit College"/>
+        <s v="Benedictine College"/>
+        <s v="Berea College"/>
+        <s v="Bryn Mawr College"/>
+        <s v="Bucknell University"/>
+        <s v="Carleton College"/>
+        <s v="Centre College"/>
+        <s v="Colby College"/>
+        <s v="Colorado College"/>
+        <s v="Connecticut College"/>
+        <s v="Denison University"/>
+        <s v="Dickinson College"/>
+        <s v="Drew University"/>
+        <s v="Earlham College"/>
+        <s v="Emerson College"/>
+        <s v="Furman University"/>
+        <s v="Gettysburg College"/>
+        <s v="Goshen College"/>
+        <s v="Grinnell College"/>
+        <s v="Guilford College"/>
+        <s v="Gustavus Adolphus College"/>
+        <s v="Hamilton College"/>
+        <s v="Harvey Mudd College"/>
+        <s v="Haverford College"/>
+        <s v="Hiram College"/>
+        <s v="Hobart and William Smith Colleges"/>
+        <s v="Illinois College"/>
+        <s v="Illinois Wesleyan University"/>
+        <s v="Juniata College"/>
+        <s v="Kalamazoo College"/>
+        <s v="Knox College"/>
+        <s v="Lake Forest College"/>
+        <s v="Lawrence University"/>
+        <s v="Lebanon Valley College"/>
+        <s v="Linfield College"/>
+        <s v="Luther College"/>
+        <s v="Macalester College"/>
+        <s v="Mills College"/>
+        <s v="Millsaps College"/>
+        <s v="Muhlenberg College"/>
+        <s v="Occidental College"/>
+        <s v="Oxford College of Emory University"/>
+        <s v="Principia College"/>
+        <s v="Reed College"/>
+        <s v="Saint Mary's College"/>
+        <s v="Saint Vincent College"/>
+        <s v="Scripps College"/>
+        <s v="Sewanee The University of the South"/>
+        <s v="Smith College"/>
+        <s v="Southwestern University"/>
+        <s v="St Lawrence University"/>
+        <s v="Susquehanna University"/>
+        <s v="Transylvania University"/>
+        <s v="Trinity University"/>
+        <s v="Union College-Schenectady"/>
+        <s v="University of Portland"/>
+        <s v="University of Puget Sound"/>
+        <s v="University of Scranton"/>
+        <s v="Vassar College"/>
+        <s v="Wabash College"/>
+        <s v="Washington and Lee University"/>
+        <s v="Whitman College"/>
+        <s v="Willamette University"/>
+        <s v="Wittenberg University"/>
+        <s v="Wofford College"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Alt name" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="ACE" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="180" maxValue="7072"/>
+    </cacheField>
+    <cacheField name="count name in Shulav data" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="2"/>
+    </cacheField>
+    <cacheField name="apostrophe" numFmtId="0">
+      <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="11" maxValue="11"/>
+    </cacheField>
+    <cacheField name="UnitID" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="115409" maxValue="487092" count="70">
+        <n v="138600"/>
+        <n v="168546"/>
+        <n v="210669"/>
+        <n v="168591"/>
+        <n v="219709"/>
+        <n v="238333"/>
+        <n v="154712"/>
+        <n v="156295"/>
+        <n v="211273"/>
+        <n v="211291"/>
+        <n v="173258"/>
+        <n v="156408"/>
+        <n v="161086"/>
+        <n v="126678"/>
+        <n v="128902"/>
+        <n v="202523"/>
+        <n v="212009"/>
+        <n v="184348"/>
+        <n v="150455"/>
+        <n v="165662"/>
+        <n v="218070"/>
+        <n v="212674"/>
+        <n v="150668"/>
+        <n v="153384"/>
+        <n v="198613"/>
+        <n v="173647"/>
+        <n v="191515"/>
+        <n v="115409"/>
+        <n v="212911"/>
+        <n v="203128"/>
+        <n v="191630"/>
+        <n v="145691"/>
+        <n v="145646"/>
+        <n v="213251"/>
+        <n v="170532"/>
+        <n v="146427"/>
+        <n v="146481"/>
+        <n v="239017"/>
+        <n v="213507"/>
+        <n v="209065"/>
+        <n v="153834"/>
+        <n v="173902"/>
+        <n v="118888"/>
+        <n v="175980"/>
+        <n v="214175"/>
+        <n v="120254"/>
+        <n v="487092"/>
+        <n v="148016"/>
+        <n v="209922"/>
+        <n v="152390"/>
+        <n v="215798"/>
+        <n v="123165"/>
+        <n v="221519"/>
+        <n v="167835"/>
+        <n v="228343"/>
+        <n v="195216"/>
+        <n v="216278"/>
+        <n v="157818"/>
+        <n v="229267"/>
+        <n v="196866"/>
+        <n v="209825"/>
+        <n v="236328"/>
+        <n v="215929"/>
+        <n v="197133"/>
+        <n v="152673"/>
+        <n v="234207"/>
+        <n v="237057"/>
+        <n v="210401"/>
+        <n v="206525"/>
+        <n v="218973"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="BASIC2018" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="22"/>
+    </cacheField>
+    <cacheField name="CC" numFmtId="0">
+      <sharedItems count="7">
+        <s v="Baccalaureate Colleges: Arts &amp; Sciences Focus"/>
+        <s v="Baccalaureate Colleges: Diverse Fields"/>
+        <s v="Doctoral/Professional Universities"/>
+        <s v="Master's Colleges &amp; Universities: Larger Programs"/>
+        <s v="Master's Colleges &amp; Universities: Small Programs"/>
+        <s v="Master's Colleges &amp; Universities: Medium Programs"/>
+        <s v="Associate's Colleges: High Transfer-High Traditional"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="70">
+  <r>
+    <x v="0"/>
+    <m/>
+    <n v="494"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="0"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <m/>
+    <n v="1244"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="1"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <m/>
+    <n v="2233"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="2"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <m/>
+    <n v="1245"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="3"/>
+    <n v="22"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <m/>
+    <n v="2519"/>
+    <n v="0"/>
+    <s v="N"/>
+    <x v="4"/>
+    <n v="17"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <m/>
+    <n v="2931"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="5"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <m/>
+    <n v="7072"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="6"/>
+    <n v="22"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <m/>
+    <n v="948"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="7"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <m/>
+    <n v="2236"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="8"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <m/>
+    <n v="2237"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="9"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <m/>
+    <n v="1327"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="10"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <m/>
+    <n v="956"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="11"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <m/>
+    <n v="1044"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="12"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <m/>
+    <n v="319"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="13"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <m/>
+    <n v="359"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="14"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <m/>
+    <n v="2065"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="15"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <m/>
+    <n v="2247"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="16"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <m/>
+    <n v="1646"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="17"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <m/>
+    <n v="753"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="18"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <m/>
+    <n v="1157"/>
+    <n v="0"/>
+    <s v="N"/>
+    <x v="19"/>
+    <n v="18"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <s v="Furman"/>
+    <n v="2446"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="20"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="21"/>
+    <m/>
+    <n v="2263"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="21"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <m/>
+    <n v="758"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="22"/>
+    <n v="22"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="23"/>
+    <m/>
+    <n v="834"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="23"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="24"/>
+    <m/>
+    <n v="1953"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="24"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="25"/>
+    <m/>
+    <n v="1338"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="25"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="26"/>
+    <m/>
+    <n v="1776"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="26"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="27"/>
+    <m/>
+    <n v="180"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="27"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="28"/>
+    <m/>
+    <n v="2267"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="28"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="29"/>
+    <m/>
+    <n v="2072"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="29"/>
+    <n v="22"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="30"/>
+    <s v="Hobart William Smith Colleges"/>
+    <n v="1755"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="30"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="31"/>
+    <m/>
+    <n v="642"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="31"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="32"/>
+    <m/>
+    <n v="646"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="32"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="33"/>
+    <m/>
+    <n v="2272"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="33"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="34"/>
+    <m/>
+    <n v="1272"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="34"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="35"/>
+    <m/>
+    <n v="652"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="35"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="36"/>
+    <m/>
+    <n v="653"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="36"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="37"/>
+    <m/>
+    <n v="2947"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="37"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="38"/>
+    <m/>
+    <n v="2277"/>
+    <n v="0"/>
+    <s v="N"/>
+    <x v="38"/>
+    <n v="20"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="39"/>
+    <s v="Linfield College-McMinnville Campus"/>
+    <n v="2195"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="39"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="40"/>
+    <m/>
+    <n v="841"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="40"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="41"/>
+    <m/>
+    <n v="1344"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="41"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="42"/>
+    <m/>
+    <n v="199"/>
+    <n v="0"/>
+    <s v="N"/>
+    <x v="42"/>
+    <n v="19"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="43"/>
+    <m/>
+    <n v="1412"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="43"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="44"/>
+    <m/>
+    <n v="2293"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="44"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="45"/>
+    <m/>
+    <n v="207"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="45"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="46"/>
+    <m/>
+    <n v="4892"/>
+    <n v="0"/>
+    <s v="N"/>
+    <x v="46"/>
+    <n v="1"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="47"/>
+    <m/>
+    <n v="683"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="47"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="48"/>
+    <m/>
+    <n v="2209"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="48"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="49"/>
+    <s v="Saint Marys College"/>
+    <n v="781"/>
+    <n v="1"/>
+    <n v="11"/>
+    <x v="49"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="50"/>
+    <m/>
+    <n v="2315"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="50"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="51"/>
+    <m/>
+    <n v="246"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="51"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="52"/>
+    <s v="Sewanee-The University of the South"/>
+    <n v="2564"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="52"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="53"/>
+    <m/>
+    <n v="1189"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="53"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="54"/>
+    <m/>
+    <n v="2664"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="54"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="55"/>
+    <m/>
+    <n v="1846"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="55"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="56"/>
+    <m/>
+    <n v="2335"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="56"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="57"/>
+    <m/>
+    <n v="981"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="57"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="58"/>
+    <m/>
+    <n v="2685"/>
+    <n v="0"/>
+    <s v="N"/>
+    <x v="58"/>
+    <n v="20"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="59"/>
+    <s v="Union College"/>
+    <n v="1884"/>
+    <n v="2"/>
+    <s v="N"/>
+    <x v="59"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="60"/>
+    <m/>
+    <n v="2213"/>
+    <n v="0"/>
+    <s v="N"/>
+    <x v="60"/>
+    <n v="19"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="61"/>
+    <m/>
+    <n v="2844"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="61"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="62"/>
+    <m/>
+    <n v="2343"/>
+    <n v="0"/>
+    <s v="N"/>
+    <x v="62"/>
+    <n v="18"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="63"/>
+    <m/>
+    <n v="1891"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="63"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="64"/>
+    <m/>
+    <n v="789"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="64"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="65"/>
+    <m/>
+    <n v="2829"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="65"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="66"/>
+    <m/>
+    <n v="2867"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="66"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="67"/>
+    <m/>
+    <n v="2215"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="67"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="68"/>
+    <m/>
+    <n v="2113"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="68"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="69"/>
+    <m/>
+    <n v="2463"/>
+    <n v="1"/>
+    <s v="N"/>
+    <x v="69"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{63A4FB75-0C78-4749-B53F-FB4D76C73A97}" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B23" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="8">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="71">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="51"/>
+        <item x="52"/>
+        <item x="53"/>
+        <item x="54"/>
+        <item x="55"/>
+        <item x="56"/>
+        <item x="57"/>
+        <item x="58"/>
+        <item x="59"/>
+        <item x="60"/>
+        <item x="61"/>
+        <item x="62"/>
+        <item x="63"/>
+        <item x="64"/>
+        <item x="65"/>
+        <item x="66"/>
+        <item x="67"/>
+        <item x="68"/>
+        <item x="69"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0">
+      <items count="71">
+        <item x="27"/>
+        <item x="42"/>
+        <item x="45"/>
+        <item x="51"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="0"/>
+        <item x="32"/>
+        <item x="31"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="47"/>
+        <item x="18"/>
+        <item x="22"/>
+        <item x="49"/>
+        <item x="64"/>
+        <item x="23"/>
+        <item x="40"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="11"/>
+        <item x="57"/>
+        <item x="12"/>
+        <item x="19"/>
+        <item x="53"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="34"/>
+        <item x="10"/>
+        <item x="25"/>
+        <item x="41"/>
+        <item x="43"/>
+        <item x="17"/>
+        <item x="26"/>
+        <item x="30"/>
+        <item x="55"/>
+        <item x="59"/>
+        <item x="63"/>
+        <item x="24"/>
+        <item x="15"/>
+        <item x="29"/>
+        <item x="68"/>
+        <item x="39"/>
+        <item x="60"/>
+        <item x="48"/>
+        <item x="67"/>
+        <item x="2"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="16"/>
+        <item x="21"/>
+        <item x="28"/>
+        <item x="33"/>
+        <item x="38"/>
+        <item x="44"/>
+        <item x="50"/>
+        <item x="62"/>
+        <item x="56"/>
+        <item x="20"/>
+        <item x="69"/>
+        <item x="4"/>
+        <item x="52"/>
+        <item x="54"/>
+        <item x="58"/>
+        <item x="65"/>
+        <item x="61"/>
+        <item x="66"/>
+        <item x="5"/>
+        <item x="37"/>
+        <item x="46"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="8">
+        <item x="6"/>
+        <item sd="0" x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="7"/>
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="20">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="46"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="22"/>
+    </i>
+    <i r="1">
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i r="1">
+      <x v="62"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="42"/>
+    </i>
+    <i r="1">
+      <x v="60"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="38"/>
+    </i>
+    <i r="1">
+      <x v="58"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of UnitID" fld="5" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -623,33 +1830,234 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0311A36A-FFF3-3642-A43D-0065441DE3F1}">
+  <dimension ref="A3:B23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" s="5">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{539942CD-20AB-7A47-9E18-D860E5EF0606}">
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.6640625" customWidth="1"/>
-    <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="40.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>73</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -657,10 +2065,22 @@
         <v>494</v>
       </c>
       <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2">
         <v>138600</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>66</v>
       </c>
@@ -668,10 +2088,22 @@
         <v>1244</v>
       </c>
       <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3">
         <v>168546</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -679,10 +2111,22 @@
         <v>2233</v>
       </c>
       <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4">
         <v>210669</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -690,10 +2134,22 @@
         <v>1245</v>
       </c>
       <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5">
         <v>168591</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>59</v>
       </c>
@@ -701,10 +2157,22 @@
         <v>2519</v>
       </c>
       <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6">
         <v>219709</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <v>17</v>
+      </c>
+      <c r="H6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>60</v>
       </c>
@@ -712,10 +2180,22 @@
         <v>2931</v>
       </c>
       <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7">
         <v>238333</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>21</v>
+      </c>
+      <c r="H7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -723,10 +2203,22 @@
         <v>7072</v>
       </c>
       <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8">
         <v>154712</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>22</v>
+      </c>
+      <c r="H8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -734,10 +2226,22 @@
         <v>948</v>
       </c>
       <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9">
         <v>156295</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <v>21</v>
+      </c>
+      <c r="H9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -745,10 +2249,22 @@
         <v>2236</v>
       </c>
       <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>93</v>
+      </c>
+      <c r="F10">
         <v>211273</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G10">
+        <v>21</v>
+      </c>
+      <c r="H10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -756,10 +2272,22 @@
         <v>2237</v>
       </c>
       <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11">
         <v>211291</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G11">
+        <v>21</v>
+      </c>
+      <c r="H11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -767,10 +2295,22 @@
         <v>1327</v>
       </c>
       <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12">
         <v>173258</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <v>21</v>
+      </c>
+      <c r="H12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -778,10 +2318,22 @@
         <v>956</v>
       </c>
       <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>93</v>
+      </c>
+      <c r="F13">
         <v>156408</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G13">
+        <v>21</v>
+      </c>
+      <c r="H13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -789,10 +2341,22 @@
         <v>1044</v>
       </c>
       <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>93</v>
+      </c>
+      <c r="F14">
         <v>161086</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <v>21</v>
+      </c>
+      <c r="H14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -800,10 +2364,22 @@
         <v>319</v>
       </c>
       <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>93</v>
+      </c>
+      <c r="F15">
         <v>126678</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G15">
+        <v>21</v>
+      </c>
+      <c r="H15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -811,10 +2387,22 @@
         <v>359</v>
       </c>
       <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>93</v>
+      </c>
+      <c r="F16">
         <v>128902</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <v>21</v>
+      </c>
+      <c r="H16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -822,10 +2410,22 @@
         <v>2065</v>
       </c>
       <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>93</v>
+      </c>
+      <c r="F17">
         <v>202523</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G17">
+        <v>21</v>
+      </c>
+      <c r="H17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -833,10 +2433,22 @@
         <v>2247</v>
       </c>
       <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>93</v>
+      </c>
+      <c r="F18">
         <v>212009</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <v>21</v>
+      </c>
+      <c r="H18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -844,10 +2456,22 @@
         <v>1646</v>
       </c>
       <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>93</v>
+      </c>
+      <c r="F19">
         <v>184348</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G19">
+        <v>21</v>
+      </c>
+      <c r="H19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -855,10 +2479,22 @@
         <v>753</v>
       </c>
       <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>93</v>
+      </c>
+      <c r="F20">
         <v>150455</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G20">
+        <v>21</v>
+      </c>
+      <c r="H20" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>53</v>
       </c>
@@ -866,24 +2502,48 @@
         <v>1157</v>
       </c>
       <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F21">
         <v>165662</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G21">
+        <v>18</v>
+      </c>
+      <c r="H21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C22">
         <v>2446</v>
       </c>
       <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>93</v>
+      </c>
+      <c r="F22">
         <v>218070</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G22">
+        <v>21</v>
+      </c>
+      <c r="H22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -891,10 +2551,22 @@
         <v>2263</v>
       </c>
       <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>93</v>
+      </c>
+      <c r="F23">
         <v>212674</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G23">
+        <v>21</v>
+      </c>
+      <c r="H23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -902,10 +2574,22 @@
         <v>758</v>
       </c>
       <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>93</v>
+      </c>
+      <c r="F24">
         <v>150668</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G24">
+        <v>22</v>
+      </c>
+      <c r="H24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -913,10 +2597,22 @@
         <v>834</v>
       </c>
       <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>93</v>
+      </c>
+      <c r="F25">
         <v>153384</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G25">
+        <v>21</v>
+      </c>
+      <c r="H25" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -924,10 +2620,22 @@
         <v>1953</v>
       </c>
       <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>93</v>
+      </c>
+      <c r="F26">
         <v>198613</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G26">
+        <v>21</v>
+      </c>
+      <c r="H26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -935,10 +2643,22 @@
         <v>1338</v>
       </c>
       <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>93</v>
+      </c>
+      <c r="F27">
         <v>173647</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G27">
+        <v>21</v>
+      </c>
+      <c r="H27" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -946,10 +2666,22 @@
         <v>1776</v>
       </c>
       <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>93</v>
+      </c>
+      <c r="F28">
         <v>191515</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G28">
+        <v>21</v>
+      </c>
+      <c r="H28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -957,10 +2689,22 @@
         <v>180</v>
       </c>
       <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>93</v>
+      </c>
+      <c r="F29">
         <v>115409</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G29">
+        <v>21</v>
+      </c>
+      <c r="H29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -968,10 +2712,22 @@
         <v>2267</v>
       </c>
       <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>93</v>
+      </c>
+      <c r="F30">
         <v>212911</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G30">
+        <v>21</v>
+      </c>
+      <c r="H30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -979,10 +2735,22 @@
         <v>2072</v>
       </c>
       <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>93</v>
+      </c>
+      <c r="F31">
         <v>203128</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G31">
+        <v>22</v>
+      </c>
+      <c r="H31" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>68</v>
       </c>
@@ -993,10 +2761,22 @@
         <v>1755</v>
       </c>
       <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>93</v>
+      </c>
+      <c r="F32">
         <v>191630</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G32">
+        <v>21</v>
+      </c>
+      <c r="H32" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -1004,10 +2784,22 @@
         <v>642</v>
       </c>
       <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>93</v>
+      </c>
+      <c r="F33">
         <v>145691</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G33">
+        <v>21</v>
+      </c>
+      <c r="H33" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>46</v>
       </c>
@@ -1015,10 +2807,22 @@
         <v>646</v>
       </c>
       <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>93</v>
+      </c>
+      <c r="F34">
         <v>145646</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G34">
+        <v>21</v>
+      </c>
+      <c r="H34" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>69</v>
       </c>
@@ -1026,10 +2830,22 @@
         <v>2272</v>
       </c>
       <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>93</v>
+      </c>
+      <c r="F35">
         <v>213251</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G35">
+        <v>21</v>
+      </c>
+      <c r="H35" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -1037,10 +2853,22 @@
         <v>1272</v>
       </c>
       <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
+        <v>93</v>
+      </c>
+      <c r="F36">
         <v>170532</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G36">
+        <v>21</v>
+      </c>
+      <c r="H36" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -1048,10 +2876,22 @@
         <v>652</v>
       </c>
       <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>93</v>
+      </c>
+      <c r="F37">
         <v>146427</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G37">
+        <v>21</v>
+      </c>
+      <c r="H37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -1059,10 +2899,22 @@
         <v>653</v>
       </c>
       <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38" t="s">
+        <v>93</v>
+      </c>
+      <c r="F38">
         <v>146481</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G38">
+        <v>21</v>
+      </c>
+      <c r="H38" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1070,10 +2922,22 @@
         <v>2947</v>
       </c>
       <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39" t="s">
+        <v>93</v>
+      </c>
+      <c r="F39">
         <v>239017</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G39">
+        <v>21</v>
+      </c>
+      <c r="H39" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>56</v>
       </c>
@@ -1081,24 +2945,48 @@
         <v>2277</v>
       </c>
       <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40" t="s">
+        <v>93</v>
+      </c>
+      <c r="F40">
         <v>213507</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G40">
+        <v>20</v>
+      </c>
+      <c r="H40" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>70</v>
       </c>
       <c r="B41" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C41">
         <v>2195</v>
       </c>
       <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41" t="s">
+        <v>93</v>
+      </c>
+      <c r="F41">
         <v>209065</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G41">
+        <v>21</v>
+      </c>
+      <c r="H41" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>11</v>
       </c>
@@ -1106,10 +2994,22 @@
         <v>841</v>
       </c>
       <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42" t="s">
+        <v>93</v>
+      </c>
+      <c r="F42">
         <v>153834</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G42">
+        <v>21</v>
+      </c>
+      <c r="H42" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -1117,10 +3017,22 @@
         <v>1344</v>
       </c>
       <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43" t="s">
+        <v>93</v>
+      </c>
+      <c r="F43">
         <v>173902</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G43">
+        <v>21</v>
+      </c>
+      <c r="H43" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>1</v>
       </c>
@@ -1128,10 +3040,22 @@
         <v>199</v>
       </c>
       <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44" t="s">
+        <v>93</v>
+      </c>
+      <c r="F44">
         <v>118888</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G44">
+        <v>19</v>
+      </c>
+      <c r="H44" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -1139,10 +3063,22 @@
         <v>1412</v>
       </c>
       <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45" t="s">
+        <v>93</v>
+      </c>
+      <c r="F45">
         <v>175980</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G45">
+        <v>21</v>
+      </c>
+      <c r="H45" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>57</v>
       </c>
@@ -1150,10 +3086,22 @@
         <v>2293</v>
       </c>
       <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46" t="s">
+        <v>93</v>
+      </c>
+      <c r="F46">
         <v>214175</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G46">
+        <v>21</v>
+      </c>
+      <c r="H46" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>2</v>
       </c>
@@ -1161,10 +3109,22 @@
         <v>207</v>
       </c>
       <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47" t="s">
+        <v>93</v>
+      </c>
+      <c r="F47">
         <v>120254</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G47">
+        <v>21</v>
+      </c>
+      <c r="H47" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>39</v>
       </c>
@@ -1172,10 +3132,22 @@
         <v>4892</v>
       </c>
       <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48" t="s">
+        <v>93</v>
+      </c>
+      <c r="F48">
         <v>487092</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="H48" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -1183,10 +3155,22 @@
         <v>683</v>
       </c>
       <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49" t="s">
+        <v>93</v>
+      </c>
+      <c r="F49">
         <v>148016</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G49">
+        <v>21</v>
+      </c>
+      <c r="H49" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>24</v>
       </c>
@@ -1194,10 +3178,22 @@
         <v>2209</v>
       </c>
       <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50" t="s">
+        <v>93</v>
+      </c>
+      <c r="F50">
         <v>209922</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G50">
+        <v>21</v>
+      </c>
+      <c r="H50" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>8</v>
       </c>
@@ -1208,10 +3204,22 @@
         <v>781</v>
       </c>
       <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>11</v>
+      </c>
+      <c r="F51">
         <v>152390</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G51">
+        <v>21</v>
+      </c>
+      <c r="H51" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>58</v>
       </c>
@@ -1219,10 +3227,22 @@
         <v>2315</v>
       </c>
       <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52" t="s">
+        <v>93</v>
+      </c>
+      <c r="F52">
         <v>215798</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G52">
+        <v>21</v>
+      </c>
+      <c r="H52" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>48</v>
       </c>
@@ -1230,10 +3250,22 @@
         <v>246</v>
       </c>
       <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53" t="s">
+        <v>93</v>
+      </c>
+      <c r="F53">
         <v>123165</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G53">
+        <v>21</v>
+      </c>
+      <c r="H53" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>72</v>
       </c>
@@ -1244,10 +3276,22 @@
         <v>2564</v>
       </c>
       <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54" t="s">
+        <v>93</v>
+      </c>
+      <c r="F54">
         <v>221519</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G54">
+        <v>21</v>
+      </c>
+      <c r="H54" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>12</v>
       </c>
@@ -1255,10 +3299,22 @@
         <v>1189</v>
       </c>
       <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55" t="s">
+        <v>93</v>
+      </c>
+      <c r="F55">
         <v>167835</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G55">
+        <v>21</v>
+      </c>
+      <c r="H55" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>34</v>
       </c>
@@ -1266,10 +3322,22 @@
         <v>2664</v>
       </c>
       <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56" t="s">
+        <v>93</v>
+      </c>
+      <c r="F56">
         <v>228343</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G56">
+        <v>21</v>
+      </c>
+      <c r="H56" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>19</v>
       </c>
@@ -1277,10 +3345,22 @@
         <v>1846</v>
       </c>
       <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57" t="s">
+        <v>93</v>
+      </c>
+      <c r="F57">
         <v>195216</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G57">
+        <v>21</v>
+      </c>
+      <c r="H57" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>64</v>
       </c>
@@ -1288,10 +3368,22 @@
         <v>2335</v>
       </c>
       <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58" t="s">
+        <v>93</v>
+      </c>
+      <c r="F58">
         <v>216278</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G58">
+        <v>21</v>
+      </c>
+      <c r="H58" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>62</v>
       </c>
@@ -1299,10 +3391,22 @@
         <v>981</v>
       </c>
       <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59" t="s">
+        <v>93</v>
+      </c>
+      <c r="F59">
         <v>157818</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G59">
+        <v>21</v>
+      </c>
+      <c r="H59" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>44</v>
       </c>
@@ -1310,24 +3414,48 @@
         <v>2685</v>
       </c>
       <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60" t="s">
+        <v>93</v>
+      </c>
+      <c r="F60">
         <v>229267</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="G60">
+        <v>20</v>
+      </c>
+      <c r="H60" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>43</v>
       </c>
       <c r="B61" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C61">
         <v>1884</v>
       </c>
-      <c r="D61" s="1">
+      <c r="D61">
+        <v>2</v>
+      </c>
+      <c r="E61" t="s">
+        <v>93</v>
+      </c>
+      <c r="F61" s="1">
         <v>196866</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G61">
+        <v>21</v>
+      </c>
+      <c r="H61" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>55</v>
       </c>
@@ -1335,10 +3463,22 @@
         <v>2213</v>
       </c>
       <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62" t="s">
+        <v>93</v>
+      </c>
+      <c r="F62">
         <v>209825</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G62">
+        <v>19</v>
+      </c>
+      <c r="H62" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>36</v>
       </c>
@@ -1346,10 +3486,22 @@
         <v>2844</v>
       </c>
       <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63" t="s">
+        <v>93</v>
+      </c>
+      <c r="F63">
         <v>236328</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G63">
+        <v>21</v>
+      </c>
+      <c r="H63" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>47</v>
       </c>
@@ -1357,10 +3509,22 @@
         <v>2343</v>
       </c>
       <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64" t="s">
+        <v>93</v>
+      </c>
+      <c r="F64">
         <v>215929</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G64">
+        <v>18</v>
+      </c>
+      <c r="H64" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>20</v>
       </c>
@@ -1368,10 +3532,22 @@
         <v>1891</v>
       </c>
       <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65" t="s">
+        <v>93</v>
+      </c>
+      <c r="F65">
         <v>197133</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G65">
+        <v>21</v>
+      </c>
+      <c r="H65" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>9</v>
       </c>
@@ -1379,10 +3555,22 @@
         <v>789</v>
       </c>
       <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66" t="s">
+        <v>93</v>
+      </c>
+      <c r="F66">
         <v>152673</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G66">
+        <v>21</v>
+      </c>
+      <c r="H66" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>35</v>
       </c>
@@ -1390,10 +3578,22 @@
         <v>2829</v>
       </c>
       <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67" t="s">
+        <v>93</v>
+      </c>
+      <c r="F67">
         <v>234207</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G67">
+        <v>21</v>
+      </c>
+      <c r="H67" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>37</v>
       </c>
@@ -1401,10 +3601,22 @@
         <v>2867</v>
       </c>
       <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68" t="s">
+        <v>93</v>
+      </c>
+      <c r="F68">
         <v>237057</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G68">
+        <v>21</v>
+      </c>
+      <c r="H68" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>25</v>
       </c>
@@ -1412,10 +3624,22 @@
         <v>2215</v>
       </c>
       <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69" t="s">
+        <v>93</v>
+      </c>
+      <c r="F69">
         <v>210401</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G69">
+        <v>21</v>
+      </c>
+      <c r="H69" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>23</v>
       </c>
@@ -1423,10 +3647,22 @@
         <v>2113</v>
       </c>
       <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70" t="s">
+        <v>93</v>
+      </c>
+      <c r="F70">
         <v>206525</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G70">
+        <v>21</v>
+      </c>
+      <c r="H70" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>32</v>
       </c>
@@ -1434,11 +3670,23 @@
         <v>2463</v>
       </c>
       <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71" t="s">
+        <v>93</v>
+      </c>
+      <c r="F71">
         <v>218973</v>
       </c>
+      <c r="G71">
+        <v>21</v>
+      </c>
+      <c r="H71" t="s">
+        <v>85</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D71" xr:uid="{BD9851F6-649C-0740-9A4C-C3F5C85C8F98}"/>
+  <autoFilter ref="A1:H1" xr:uid="{B984ADAC-0766-CF4A-890B-CDE90849422B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>